<commit_message>
Rename IntelliJ project to `main.py` and add preliminary Gantt planning file
</commit_message>
<xml_diff>
--- a/planning/gantt.xlsx
+++ b/planning/gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esteban BARRACHO\Desktop\PolyBase\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA0D44B-2678-4753-B829-1D94B1CE5227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC11FF9-B0D6-4FE9-9022-66D87F348F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>…</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>PolyBase</t>
+  </si>
+  <si>
+    <t>Conceptualisation (BD conceptuelle,…)</t>
   </si>
 </sst>
 </file>
@@ -917,7 +920,7 @@
   <dimension ref="B2:AH48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -987,7 +990,7 @@
       </c>
       <c r="D7" s="25">
         <f>SUM(D10:D36)</f>
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E7" s="17">
         <f t="shared" ref="E7:Z7" si="0">SUM(E11:E36)</f>
@@ -1247,11 +1250,11 @@
       </c>
       <c r="C9" s="19">
         <f>SUM(D9:AH9)</f>
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="D9" s="23">
         <f>SUM(D10:D46)</f>
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E9" s="23">
         <f>SUM(E10:E46)</f>
@@ -1601,12 +1604,16 @@
       <c r="AH14" s="11"/>
     </row>
     <row r="15" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="26"/>
+      <c r="B15" s="26" t="s">
+        <v>24</v>
+      </c>
       <c r="C15" s="22">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="D15" s="15"/>
+        <v>4</v>
+      </c>
+      <c r="D15" s="15">
+        <v>4</v>
+      </c>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>

</xml_diff>

<commit_message>
Extend PolyBase with new modules, static assets, and enhanced frontend/backend integration
- Added new routers for task, facture, prestation, and dashboard APIs to expand functionality.
- Introduced multiple user-facing frontend pages: `login.html`, `dashboard.html`, `agenda.html`, and `documents.html` with corresponding JavaScript and CSS for dynamic and styled interactions.
- Enhanced `main.py` with frontend route handling and reproduction of examples for `dashboard` and `task tracking`.
- Refined Dockerfile and `docker-compose.yml` for improved container setup and initialization.
</commit_message>
<xml_diff>
--- a/planning/gantt.xlsx
+++ b/planning/gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esteban BARRACHO\Desktop\PolyBase\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC11FF9-B0D6-4FE9-9022-66D87F348F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472CFD21-B4B5-4D4A-A2FB-333331C17861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -920,7 +920,7 @@
   <dimension ref="B2:AH48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -994,7 +994,7 @@
       </c>
       <c r="E7" s="17">
         <f t="shared" ref="E7:Z7" si="0">SUM(E11:E36)</f>
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F7" s="17">
         <f t="shared" si="0"/>
@@ -1250,7 +1250,7 @@
       </c>
       <c r="C9" s="19">
         <f>SUM(D9:AH9)</f>
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D9" s="23">
         <f>SUM(D10:D46)</f>
@@ -1258,7 +1258,7 @@
       </c>
       <c r="E9" s="23">
         <f>SUM(E10:E46)</f>
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F9" s="23">
         <f t="shared" ref="F9:Z9" si="12">SUM(F10:F46)</f>
@@ -1383,13 +1383,13 @@
       </c>
       <c r="C10" s="22">
         <f>SUM(D10:AH10)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D10" s="14">
         <v>3</v>
       </c>
       <c r="E10" s="14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F10" s="14">
         <v>2</v>
@@ -1431,13 +1431,13 @@
       </c>
       <c r="C11" s="22">
         <f t="shared" ref="C11:C46" si="14">SUM(D11:AH11)</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" s="15">
         <v>4</v>
       </c>
       <c r="E11" s="15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" s="15">
         <v>3</v>
@@ -1609,12 +1609,14 @@
       </c>
       <c r="C15" s="22">
         <f t="shared" si="14"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D15" s="15">
         <v>4</v>
       </c>
-      <c r="E15" s="10"/>
+      <c r="E15" s="10">
+        <v>2</v>
+      </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>

</xml_diff>

<commit_message>
Standardize SQL schema, update demo scripts, and enhance Docker configuration
- Refined SQL initialization scripts to address case-sensitivity and naming consistency (`heures_prestees`, `emise`, etc.).
- Improved demo logic in `demo_api.py` with additional data persistence (`session.commit()` added at multiple steps).
- Enhanced Docker setup to include environment variable optimizations and cleanup commands in the Dockerfile.
- Updated `docker-compose.yml` to standardize database names across services.
- Removed deprecated files and adjusted project structure to reflect updated requirements.
</commit_message>
<xml_diff>
--- a/planning/gantt.xlsx
+++ b/planning/gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esteban BARRACHO\Desktop\PolyBase\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472CFD21-B4B5-4D4A-A2FB-333331C17861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A39C86-3C35-47D0-B2C3-E12076147202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -920,7 +920,7 @@
   <dimension ref="B2:AH48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -994,7 +994,7 @@
       </c>
       <c r="E7" s="17">
         <f t="shared" ref="E7:Z7" si="0">SUM(E11:E36)</f>
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="F7" s="17">
         <f t="shared" si="0"/>
@@ -1250,7 +1250,7 @@
       </c>
       <c r="C9" s="19">
         <f>SUM(D9:AH9)</f>
-        <v>234</v>
+        <v>248</v>
       </c>
       <c r="D9" s="23">
         <f>SUM(D10:D46)</f>
@@ -1258,7 +1258,7 @@
       </c>
       <c r="E9" s="23">
         <f>SUM(E10:E46)</f>
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="F9" s="23">
         <f t="shared" ref="F9:Z9" si="12">SUM(F10:F46)</f>
@@ -1563,11 +1563,11 @@
       </c>
       <c r="C14" s="22">
         <f t="shared" si="14"/>
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="F14" s="15">
         <v>28</v>
@@ -1609,13 +1609,13 @@
       </c>
       <c r="C15" s="22">
         <f t="shared" si="14"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D15" s="15">
         <v>4</v>
       </c>
       <c r="E15" s="10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>

</xml_diff>

<commit_message>
Add comprehensive documentation, refactor schema triggers, and update specifications
- Replaced emoji triggers in `mysql-init/init.sql` with clear labels for better readability and maintainability.
- Added detailed docstrings across routers and methods for improved code documentation (`collaborateur.py`, `finance.py`, etc.).
- Introduced specifications and implementation details as comments in JavaScript and CSS files (`dashboard.js`, `agenda.css`, etc.).
- Standardized CSS comments to improve clarity and structure across multiple style files.
- Updated `admin.js` with modular enumerations, input sanitization, and type handling enhancements.
</commit_message>
<xml_diff>
--- a/planning/gantt.xlsx
+++ b/planning/gantt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esteban BARRACHO\Desktop\PolyBase\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A39C86-3C35-47D0-B2C3-E12076147202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151EA899-B382-48B5-8641-002F038E9249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>…</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>Conceptualisation (BD conceptuelle,…)</t>
+  </si>
+  <si>
+    <t>Documentation</t>
   </si>
 </sst>
 </file>
@@ -610,8 +613,8 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="5" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="20 % - Accent1" xfId="1" builtinId="30"/>
-    <cellStyle name="60 % - Accent2" xfId="3" builtinId="36"/>
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
+    <cellStyle name="60% - Accent2" xfId="3" builtinId="36"/>
     <cellStyle name="Accent2" xfId="2" builtinId="33"/>
     <cellStyle name="Accent3" xfId="4" builtinId="37"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -920,10 +923,10 @@
   <dimension ref="B2:AH48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="41.77734375" customWidth="1"/>
     <col min="3" max="3" width="21.77734375" customWidth="1"/>
@@ -990,15 +993,15 @@
       </c>
       <c r="D7" s="25">
         <f>SUM(D10:D36)</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E7" s="17">
         <f t="shared" ref="E7:Z7" si="0">SUM(E11:E36)</f>
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F7" s="17">
         <f t="shared" si="0"/>
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G7" s="17">
         <f t="shared" si="0"/>
@@ -1006,11 +1009,11 @@
       </c>
       <c r="H7" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="I7" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" si="0"/>
@@ -1250,31 +1253,31 @@
       </c>
       <c r="C9" s="19">
         <f>SUM(D9:AH9)</f>
-        <v>248</v>
+        <v>399</v>
       </c>
       <c r="D9" s="23">
         <f>SUM(D10:D46)</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E9" s="23">
         <f>SUM(E10:E46)</f>
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F9" s="23">
         <f t="shared" ref="F9:Z9" si="12">SUM(F10:F46)</f>
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G9" s="23">
         <f t="shared" si="12"/>
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="H9" s="23">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="I9" s="23">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="J9" s="23">
         <f t="shared" si="12"/>
@@ -1383,7 +1386,7 @@
       </c>
       <c r="C10" s="22">
         <f>SUM(D10:AH10)</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D10" s="14">
         <v>3</v>
@@ -1392,13 +1395,17 @@
         <v>3</v>
       </c>
       <c r="F10" s="14">
+        <v>6</v>
+      </c>
+      <c r="G10" s="14">
+        <v>8</v>
+      </c>
+      <c r="H10" s="14">
         <v>2</v>
       </c>
-      <c r="G10" s="14">
-        <v>2</v>
-      </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
+      <c r="I10" s="14">
+        <v>5</v>
+      </c>
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
       <c r="L10" s="14"/>
@@ -1431,7 +1438,7 @@
       </c>
       <c r="C11" s="22">
         <f t="shared" ref="C11:C46" si="14">SUM(D11:AH11)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D11" s="15">
         <v>4</v>
@@ -1440,13 +1447,17 @@
         <v>2</v>
       </c>
       <c r="F11" s="15">
+        <v>1</v>
+      </c>
+      <c r="G11" s="15">
+        <v>2</v>
+      </c>
+      <c r="H11" s="15">
         <v>3</v>
       </c>
-      <c r="G11" s="15">
-        <v>3</v>
-      </c>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
+      <c r="I11" s="15">
+        <v>1</v>
+      </c>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
@@ -1474,17 +1485,31 @@
       <c r="AH11" s="11"/>
     </row>
     <row r="12" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="24"/>
+      <c r="B12" s="24" t="s">
+        <v>25</v>
+      </c>
       <c r="C12" s="22">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
+        <v>21</v>
+      </c>
+      <c r="D12" s="15">
+        <v>1</v>
+      </c>
+      <c r="E12" s="10">
+        <v>1</v>
+      </c>
+      <c r="F12" s="10">
+        <v>1</v>
+      </c>
+      <c r="G12" s="10">
+        <v>1</v>
+      </c>
+      <c r="H12" s="10">
+        <v>1</v>
+      </c>
+      <c r="I12" s="10">
+        <v>16</v>
+      </c>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
@@ -1517,7 +1542,7 @@
       </c>
       <c r="C13" s="22">
         <f t="shared" si="14"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15">
@@ -1529,8 +1554,12 @@
       <c r="G13" s="15">
         <v>3</v>
       </c>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
+      <c r="H13" s="15">
+        <v>2</v>
+      </c>
+      <c r="I13" s="15">
+        <v>0</v>
+      </c>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
       <c r="L13" s="15"/>
@@ -1563,7 +1592,7 @@
       </c>
       <c r="C14" s="22">
         <f t="shared" si="14"/>
-        <v>96</v>
+        <v>148</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15">
@@ -1575,8 +1604,12 @@
       <c r="G14" s="15">
         <v>28</v>
       </c>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
+      <c r="H14" s="15">
+        <v>28</v>
+      </c>
+      <c r="I14" s="15">
+        <v>24</v>
+      </c>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
       <c r="L14" s="15"/>
@@ -1925,7 +1958,7 @@
       </c>
       <c r="C23" s="22">
         <f t="shared" si="14"/>
-        <v>84</v>
+        <v>126</v>
       </c>
       <c r="D23" s="15">
         <v>21</v>
@@ -1939,8 +1972,12 @@
       <c r="G23" s="15">
         <v>21</v>
       </c>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
+      <c r="H23" s="15">
+        <v>21</v>
+      </c>
+      <c r="I23" s="15">
+        <v>21</v>
+      </c>
       <c r="J23" s="15"/>
       <c r="K23" s="15"/>
       <c r="L23" s="15"/>
@@ -1973,7 +2010,7 @@
       </c>
       <c r="C24" s="22">
         <f t="shared" si="14"/>
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D24" s="15">
         <v>8</v>
@@ -1987,8 +2024,12 @@
       <c r="G24" s="10">
         <v>8</v>
       </c>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
+      <c r="H24" s="10">
+        <v>8</v>
+      </c>
+      <c r="I24" s="10">
+        <v>8</v>
+      </c>
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>

</xml_diff>